<commit_message>
Updates for manuscript revision
</commit_message>
<xml_diff>
--- a/Results/model_results.xlsx
+++ b/Results/model_results.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr date1904="false"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Model Summaries" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Model Estimates" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Parameter Estimates" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t xml:space="preserve">model</t>
   </si>
@@ -54,7 +54,10 @@
     <t xml:space="preserve">nobs</t>
   </si>
   <si>
-    <t xml:space="preserve">Etoh_and_smoking</t>
+    <t xml:space="preserve">Males</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Females</t>
   </si>
   <si>
     <t xml:space="preserve">term</t>
@@ -90,9 +93,6 @@
     <t xml:space="preserve">smok_cat5Regular smoker</t>
   </si>
   <si>
-    <t xml:space="preserve">sexMale</t>
-  </si>
-  <si>
     <t xml:space="preserve">age_at_survey</t>
   </si>
   <si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t xml:space="preserve">educ_levelTechnical college / technician / master</t>
+  </si>
+  <si>
+    <t xml:space="preserve">educ_levelAbitur</t>
   </si>
   <si>
     <t xml:space="preserve">educ_levelUniversity</t>
@@ -117,7 +120,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
   <fonts count="1">
     <font>
@@ -436,10 +439,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
@@ -489,40 +492,81 @@
         <v>13</v>
       </c>
       <c r="B2" t="n">
-        <v>0.0481866209137285</v>
+        <v>0.0533119027056901</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0437832138218703</v>
+        <v>0.0444579852489807</v>
       </c>
       <c r="D2" t="n">
-        <v>15.0055502442593</v>
+        <v>15.4326147813358</v>
       </c>
       <c r="E2" t="n">
-        <v>10.9430311366906</v>
+        <v>6.02127848676646</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0000000000000000000000326803450087154</v>
+        <v>0.0000000000510341712493853</v>
       </c>
       <c r="G2" t="n">
         <v>13</v>
       </c>
       <c r="H2" t="n">
-        <v>-11648.6435095615</v>
+        <v>-5827.17685708492</v>
       </c>
       <c r="I2" t="n">
-        <v>23327.2870191229</v>
+        <v>11684.3537141698</v>
       </c>
       <c r="J2" t="n">
-        <v>23416.4756631021</v>
+        <v>11763.0599229386</v>
       </c>
       <c r="K2" t="n">
-        <v>632717.972153701</v>
+        <v>331050.182594856</v>
       </c>
       <c r="L2" t="n">
-        <v>2810</v>
+        <v>1390</v>
       </c>
       <c r="M2" t="n">
-        <v>2824</v>
+        <v>1404</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.0638559977684699</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.0568741904180795</v>
+      </c>
+      <c r="D3" t="n">
+        <v>14.3070124078752</v>
+      </c>
+      <c r="E3" t="n">
+        <v>9.14605553602079</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.0000000000000000293971164399593</v>
+      </c>
+      <c r="G3" t="n">
+        <v>12</v>
+      </c>
+      <c r="H3" t="n">
+        <v>-6610.72828063101</v>
+      </c>
+      <c r="I3" t="n">
+        <v>13249.456561262</v>
+      </c>
+      <c r="J3" t="n">
+        <v>13324.9363745475</v>
+      </c>
+      <c r="K3" t="n">
+        <v>329347.181898902</v>
+      </c>
+      <c r="L3" t="n">
+        <v>1609</v>
+      </c>
+      <c r="M3" t="n">
+        <v>1622</v>
       </c>
     </row>
   </sheetData>
@@ -532,10 +576,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
@@ -544,13 +588,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
@@ -559,10 +603,10 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2">
@@ -570,25 +614,25 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C2" t="n">
-        <v>23.2569354242088</v>
+        <v>5.29333136071519</v>
       </c>
       <c r="D2" t="n">
-        <v>15.6518148856123</v>
+        <v>16.809180251152</v>
       </c>
       <c r="E2" t="n">
-        <v>1.4858938464438</v>
+        <v>0.314907168679591</v>
       </c>
       <c r="F2" t="n">
-        <v>0.137419380809358</v>
+        <v>0.752879403039063</v>
       </c>
       <c r="G2" t="n">
-        <v>-7.43327728864046</v>
+        <v>-27.6807688356121</v>
       </c>
       <c r="H2" t="n">
-        <v>53.9471481370581</v>
+        <v>38.2674315570424</v>
       </c>
     </row>
     <row r="3">
@@ -596,25 +640,25 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C3" t="n">
-        <v>0.13994222758006</v>
+        <v>0.113237786158915</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0155115396322402</v>
+        <v>0.0178410797894489</v>
       </c>
       <c r="E3" t="n">
-        <v>9.02181413953227</v>
+        <v>6.34702537600236</v>
       </c>
       <c r="F3" t="n">
-        <v>0.000000000000000000334557947808205</v>
+        <v>0.000000000296465376974968</v>
       </c>
       <c r="G3" t="n">
-        <v>0.109527067785725</v>
+        <v>0.0782394374115014</v>
       </c>
       <c r="H3" t="n">
-        <v>0.170357387374395</v>
+        <v>0.148236134906329</v>
       </c>
     </row>
     <row r="4">
@@ -622,25 +666,25 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C4" t="n">
-        <v>1.11369204145529</v>
+        <v>3.47477401755889</v>
       </c>
       <c r="D4" t="n">
-        <v>1.03519377340025</v>
+        <v>1.59045777468678</v>
       </c>
       <c r="E4" t="n">
-        <v>1.07582954039339</v>
+        <v>2.18476345166926</v>
       </c>
       <c r="F4" t="n">
-        <v>0.282095857683281</v>
+        <v>0.0290727337511521</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.916124777671236</v>
+        <v>0.354817348823949</v>
       </c>
       <c r="H4" t="n">
-        <v>3.14350886058181</v>
+        <v>6.59473068629383</v>
       </c>
     </row>
     <row r="5">
@@ -648,25 +692,25 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C5" t="n">
-        <v>1.20048763900494</v>
+        <v>0.747932910436062</v>
       </c>
       <c r="D5" t="n">
-        <v>0.66547084322633</v>
+        <v>0.961957574544779</v>
       </c>
       <c r="E5" t="n">
-        <v>1.80396729807837</v>
+        <v>0.77751132713935</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0713434828937519</v>
+        <v>0.436989461344672</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.104373291313702</v>
+        <v>-1.13911244059951</v>
       </c>
       <c r="H5" t="n">
-        <v>2.50534856932358</v>
+        <v>2.63497826147164</v>
       </c>
     </row>
     <row r="6">
@@ -674,25 +718,25 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C6" t="n">
-        <v>3.10775162474799</v>
+        <v>4.4398065829523</v>
       </c>
       <c r="D6" t="n">
-        <v>2.21606046674354</v>
+        <v>2.91271718463475</v>
       </c>
       <c r="E6" t="n">
-        <v>1.40237672725364</v>
+        <v>1.52428344446666</v>
       </c>
       <c r="F6" t="n">
-        <v>0.160913241581242</v>
+        <v>0.127665395262149</v>
       </c>
       <c r="G6" t="n">
-        <v>-1.23751872287245</v>
+        <v>-1.2739895007757</v>
       </c>
       <c r="H6" t="n">
-        <v>7.45302197236842</v>
+        <v>10.1536026666803</v>
       </c>
     </row>
     <row r="7">
@@ -700,25 +744,25 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C7" t="n">
-        <v>2.85479242471704</v>
+        <v>4.68426062357128</v>
       </c>
       <c r="D7" t="n">
-        <v>0.920956083831771</v>
+        <v>1.40476429439318</v>
       </c>
       <c r="E7" t="n">
-        <v>3.09981385088338</v>
+        <v>3.33455273761408</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0019556023566876</v>
+        <v>0.000876872747098563</v>
       </c>
       <c r="G7" t="n">
-        <v>1.04897384594179</v>
+        <v>1.92857367730459</v>
       </c>
       <c r="H7" t="n">
-        <v>4.66061100349229</v>
+        <v>7.43994756983796</v>
       </c>
     </row>
     <row r="8">
@@ -726,25 +770,25 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.662298863926348</v>
+        <v>0.276317934426404</v>
       </c>
       <c r="D8" t="n">
-        <v>0.623790435989378</v>
+        <v>0.0767977202162969</v>
       </c>
       <c r="E8" t="n">
-        <v>-1.06173295663934</v>
+        <v>3.59799657656723</v>
       </c>
       <c r="F8" t="n">
-        <v>0.28844817392845</v>
+        <v>0.000331928287259142</v>
       </c>
       <c r="G8" t="n">
-        <v>-1.88543249466927</v>
+        <v>0.125665988083683</v>
       </c>
       <c r="H8" t="n">
-        <v>0.560834766816569</v>
+        <v>0.426969880769125</v>
       </c>
     </row>
     <row r="9">
@@ -752,25 +796,25 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C9" t="n">
-        <v>0.12153014204647</v>
+        <v>-0.0953909786765939</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0524073766995209</v>
+        <v>0.0929649142098184</v>
       </c>
       <c r="E9" t="n">
-        <v>2.31895106567281</v>
+        <v>-1.02609656005598</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0204690798309804</v>
+        <v>0.305024600151243</v>
       </c>
       <c r="G9" t="n">
-        <v>0.0187693088533045</v>
+        <v>-0.277757658675009</v>
       </c>
       <c r="H9" t="n">
-        <v>0.224290975239636</v>
+        <v>0.0869757013218209</v>
       </c>
     </row>
     <row r="10">
@@ -778,25 +822,25 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.229977489537463</v>
+        <v>2.42666003318875</v>
       </c>
       <c r="D10" t="n">
-        <v>0.054438944247808</v>
+        <v>15.9596554273863</v>
       </c>
       <c r="E10" t="n">
-        <v>-4.22450311472974</v>
+        <v>0.15204965071017</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0000247087641527234</v>
+        <v>0.879169840929234</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.336721837783236</v>
+        <v>-28.8809510042636</v>
       </c>
       <c r="H10" t="n">
-        <v>-0.123233141291691</v>
+        <v>33.7342710706411</v>
       </c>
     </row>
     <row r="11">
@@ -804,25 +848,25 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C11" t="n">
-        <v>-2.45980968925682</v>
+        <v>5.66355371981544</v>
       </c>
       <c r="D11" t="n">
-        <v>15.1265024784824</v>
+        <v>15.5336572744265</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.162615891727511</v>
+        <v>0.36459885909415</v>
       </c>
       <c r="F11" t="n">
-        <v>0.87083256633237</v>
+        <v>0.715466326014674</v>
       </c>
       <c r="G11" t="n">
-        <v>-32.1199853339872</v>
+        <v>-24.8083886193858</v>
       </c>
       <c r="H11" t="n">
-        <v>27.2003659554736</v>
+        <v>36.1354960590167</v>
       </c>
     </row>
     <row r="12">
@@ -830,25 +874,25 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C12" t="n">
-        <v>1.21619004893257</v>
+        <v>4.29614047481476</v>
       </c>
       <c r="D12" t="n">
-        <v>15.0517482780619</v>
+        <v>15.5660212081408</v>
       </c>
       <c r="E12" t="n">
-        <v>0.0808005838567723</v>
+        <v>0.275994772033842</v>
       </c>
       <c r="F12" t="n">
-        <v>0.935606297837962</v>
+        <v>0.782593108311736</v>
       </c>
       <c r="G12" t="n">
-        <v>-28.2974069192129</v>
+        <v>-26.2392892907272</v>
       </c>
       <c r="H12" t="n">
-        <v>30.7297870170781</v>
+        <v>34.8315702403567</v>
       </c>
     </row>
     <row r="13">
@@ -856,25 +900,25 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C13" t="n">
-        <v>1.53852085719175</v>
+        <v>7.5602729996053</v>
       </c>
       <c r="D13" t="n">
-        <v>15.064283143755</v>
+        <v>15.5521223824365</v>
       </c>
       <c r="E13" t="n">
-        <v>0.102130373049285</v>
+        <v>0.486124839664545</v>
       </c>
       <c r="F13" t="n">
-        <v>0.918660479883505</v>
+        <v>0.626955282996558</v>
       </c>
       <c r="G13" t="n">
-        <v>-27.9996545829878</v>
+        <v>-22.9478918271034</v>
       </c>
       <c r="H13" t="n">
-        <v>31.0766962973713</v>
+        <v>38.068437826314</v>
       </c>
     </row>
     <row r="14">
@@ -882,25 +926,25 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C14" t="n">
-        <v>2.92007992403994</v>
+        <v>4.20148907317058</v>
       </c>
       <c r="D14" t="n">
-        <v>15.0635654065974</v>
+        <v>15.6094242954748</v>
       </c>
       <c r="E14" t="n">
-        <v>0.193850515812214</v>
+        <v>0.269163615110942</v>
       </c>
       <c r="F14" t="n">
-        <v>0.846306942671575</v>
+        <v>0.787843725329472</v>
       </c>
       <c r="G14" t="n">
-        <v>-26.6166881709724</v>
+        <v>-26.4190833185554</v>
       </c>
       <c r="H14" t="n">
-        <v>32.4568480190523</v>
+        <v>34.8220614648966</v>
       </c>
     </row>
     <row r="15">
@@ -908,25 +952,363 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" t="n">
+        <v>5.11101407623988</v>
+      </c>
+      <c r="D15" t="n">
+        <v>15.5589641512687</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.328493209865974</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.742588256455526</v>
+      </c>
+      <c r="G15" t="n">
+        <v>-25.4105720576131</v>
+      </c>
+      <c r="H15" t="n">
+        <v>35.6326002100929</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" t="n">
+        <v>30.4499099783251</v>
+      </c>
+      <c r="D16" t="n">
+        <v>5.10902068914304</v>
+      </c>
+      <c r="E16" t="n">
+        <v>5.96002870824792</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.00000000309267038358885</v>
+      </c>
+      <c r="G16" t="n">
+        <v>20.4288752398763</v>
+      </c>
+      <c r="H16" t="n">
+        <v>40.4709447167738</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.228322918891214</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.0293875122668693</v>
+      </c>
+      <c r="E17" t="n">
+        <v>7.76938574513567</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.0000000000000139550232729419</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.170681092948191</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.285964744834237</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" t="n">
+        <v>-0.248597156307385</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1.25793878202011</v>
+      </c>
+      <c r="E18" t="n">
+        <v>-0.197622618732022</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.843365298871899</v>
+      </c>
+      <c r="G18" t="n">
+        <v>-2.71596791099108</v>
+      </c>
+      <c r="H18" t="n">
+        <v>2.21877359837631</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1.18537578073293</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.862620198596931</v>
+      </c>
+      <c r="E19" t="n">
+        <v>1.37415722778225</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.169584255971074</v>
+      </c>
+      <c r="G19" t="n">
+        <v>-0.506601508495347</v>
+      </c>
+      <c r="H19" t="n">
+        <v>2.8773530699612</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" t="n">
+        <v>2.25780992833913</v>
+      </c>
+      <c r="D20" t="n">
+        <v>3.0321148037793</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.744632071821602</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.45660291499987</v>
+      </c>
+      <c r="G20" t="n">
+        <v>-3.68949966940958</v>
+      </c>
+      <c r="H20" t="n">
+        <v>8.20511952608784</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" t="n">
+        <v>1.33412879987719</v>
+      </c>
+      <c r="D21" t="n">
+        <v>1.12849957751242</v>
+      </c>
+      <c r="E21" t="n">
+        <v>1.1822147092142</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.237295195726541</v>
+      </c>
+      <c r="G21" t="n">
+        <v>-0.879354792508407</v>
+      </c>
+      <c r="H21" t="n">
+        <v>3.54761239226279</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" t="n">
+        <v>-0.0192072251295009</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.0669066469133445</v>
+      </c>
+      <c r="E22" t="n">
+        <v>-0.287074992031473</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.774091864217458</v>
+      </c>
+      <c r="G22" t="n">
+        <v>-0.150440561955978</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.112026111696977</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" t="n">
+        <v>-0.251611075332022</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.0627095545498564</v>
+      </c>
+      <c r="E23" t="n">
+        <v>-4.01232439200286</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.0000628834611220802</v>
+      </c>
+      <c r="G23" t="n">
+        <v>-0.374612069614973</v>
+      </c>
+      <c r="H23" t="n">
+        <v>-0.128610081049072</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" t="n">
+        <v>2.87583678167169</v>
+      </c>
+      <c r="D24" t="n">
+        <v>1.78043571608051</v>
+      </c>
+      <c r="E24" t="n">
+        <v>1.61524325517498</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.10645408182697</v>
+      </c>
+      <c r="G24" t="n">
+        <v>-0.616380072789792</v>
+      </c>
+      <c r="H24" t="n">
+        <v>6.36805363613316</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" t="n">
+        <v>4.06403313488797</v>
+      </c>
+      <c r="D25" t="n">
+        <v>1.84711680898249</v>
+      </c>
+      <c r="E25" t="n">
+        <v>2.20020364447157</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.0279341484730318</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.441025354136364</v>
+      </c>
+      <c r="H25" t="n">
+        <v>7.68704091563958</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" t="n">
+        <v>3.90103786013192</v>
+      </c>
+      <c r="D26" t="n">
+        <v>1.95866602164811</v>
+      </c>
+      <c r="E26" t="n">
+        <v>1.99168097930724</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.0465748687994227</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.0592330528691005</v>
+      </c>
+      <c r="H26" t="n">
+        <v>7.74284266739474</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" t="s">
         <v>32</v>
       </c>
-      <c r="C15" t="n">
-        <v>1.57524285733945</v>
-      </c>
-      <c r="D15" t="n">
-        <v>15.0665245941294</v>
-      </c>
-      <c r="E15" t="n">
-        <v>0.10455250296762</v>
-      </c>
-      <c r="F15" t="n">
-        <v>0.916738366876136</v>
-      </c>
-      <c r="G15" t="n">
-        <v>-27.9673276379363</v>
-      </c>
-      <c r="H15" t="n">
-        <v>31.1178133526152</v>
+      <c r="C27" t="n">
+        <v>2.83329071021574</v>
+      </c>
+      <c r="D27" t="n">
+        <v>2.24932236259308</v>
+      </c>
+      <c r="E27" t="n">
+        <v>1.25961967805693</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.207989274096524</v>
+      </c>
+      <c r="G27" t="n">
+        <v>-1.57861891101848</v>
+      </c>
+      <c r="H27" t="n">
+        <v>7.24520033144997</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" t="n">
+        <v>4.19350854700612</v>
+      </c>
+      <c r="D28" t="n">
+        <v>1.97798064642134</v>
+      </c>
+      <c r="E28" t="n">
+        <v>2.12009584350242</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.0341506541422248</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0.313819272721278</v>
+      </c>
+      <c r="H28" t="n">
+        <v>8.07319782129096</v>
       </c>
     </row>
   </sheetData>

</xml_diff>